<commit_message>
add SEOS and related documentation
</commit_message>
<xml_diff>
--- a/Documentacion/MEF Funciones - Descripcion de Estados.xlsx
+++ b/Documentacion/MEF Funciones - Descripcion de Estados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Users\Agustín\Documents\MEGAsync\Facultad\2021\Segundo semestre\Taller 1\Projects\TP4\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2732A28-C249-4FC0-8C06-C6AE22AE21E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152514CF-48A4-4E71-972F-E23FF0A021D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2685" windowWidth="19440" windowHeight="15000" xr2:uid="{A2BAAD8B-E166-4723-A5A7-E8E115F14A37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A2BAAD8B-E166-4723-A5A7-E8E115F14A37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,42 +45,24 @@
     <t>Razon</t>
   </si>
   <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>Se carga el primer estado del juego</t>
   </si>
   <si>
     <t>Se alimenta el sistema</t>
   </si>
   <si>
-    <t>Ready</t>
-  </si>
-  <si>
     <t>Pausar el juego, conjelar las celulas</t>
   </si>
   <si>
-    <t xml:space="preserve">Estado por defecto. Se presiona "Start" en 4, se presiona "Sel" en 5. Se reseteó la partida en 3 </t>
-  </si>
-  <si>
     <t>Recrear el ultimo patron guardado en la sesion</t>
   </si>
   <si>
-    <t>Play</t>
-  </si>
-  <si>
     <t>Transcurrir con el juego.</t>
   </si>
   <si>
     <t>Se presiona el boton START en 2</t>
   </si>
   <si>
-    <t>Se presiona el boton A en 2</t>
-  </si>
-  <si>
     <t>Se presiona el boton SET en 2</t>
   </si>
   <si>
@@ -90,10 +72,28 @@
     <t>2, 3, 4, 5</t>
   </si>
   <si>
-    <t>Edit</t>
-  </si>
-  <si>
     <t>Se cargan distintos patrones predefinidos en un ciclo (7 en total)</t>
+  </si>
+  <si>
+    <t>Se presiona el boton RESET en 2</t>
+  </si>
+  <si>
+    <t>Estado por defecto. Se presiona START en 4.</t>
+  </si>
+  <si>
+    <t>BEGIN</t>
+  </si>
+  <si>
+    <t>READY</t>
+  </si>
+  <si>
+    <t>RESTART</t>
+  </si>
+  <si>
+    <t>PLAY</t>
+  </si>
+  <si>
+    <t>EDIT</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,16 +508,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -525,16 +525,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -542,13 +542,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4">
         <v>2</v>
@@ -559,16 +559,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -576,13 +576,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4">
         <v>2</v>

</xml_diff>